<commit_message>
-EditorSetting:Use new edtiotSetting name.
</commit_message>
<xml_diff>
--- a/Assets/Resource_SVN/Table/Hero.xlsx
+++ b/Assets/Resource_SVN/Table/Hero.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26100" windowHeight="11595"/>
+    <workbookView windowWidth="15882" windowHeight="13191"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -99,8 +99,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -110,6 +110,73 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
@@ -117,76 +184,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -216,29 +216,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
@@ -246,6 +223,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -255,7 +241,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -270,13 +270,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -288,97 +354,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -390,67 +450,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -461,6 +461,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -484,21 +523,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,32 +556,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,10 +569,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -581,34 +581,34 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -620,94 +620,94 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1040,10 +1040,10 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="I2" sqref="I$1:N$1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="3" width="11.5" customWidth="1"/>
@@ -1168,7 +1168,7 @@
         <v>21</v>
       </c>
       <c r="D5" s="1">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1">
         <v>3</v>
@@ -1194,7 +1194,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="1">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="E6" s="1">
         <v>4</v>
@@ -1251,7 +1251,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1268,7 +1268,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.509027777777778" footer="0.509027777777778"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>